<commit_message>
adjusted timing to be more reasonable
</commit_message>
<xml_diff>
--- a/input/PROP_trialText.xlsx
+++ b/input/PROP_trialText.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
   <si>
     <t>%stFile</t>
   </si>
@@ -33,9 +33,6 @@
     <t>cbt01_1</t>
   </si>
   <si>
-    <t>For example, if you feel depressed, you will likely have many negative thoughts, possibly about yourself or others or about your life in general.</t>
-  </si>
-  <si>
     <t>cbt01_2</t>
   </si>
   <si>
@@ -459,9 +456,6 @@
     <t>Also, when you're depressed, you're more likely to act in ways that feed your negative thoughts and sadness.</t>
   </si>
   <si>
-    <t>The first step in doing this is learning to catch or identify automatic thoughts. Automatic thoughts are thoughts that pop into our heads, and most of the time, they happen automatically and outside of our awareness.</t>
-  </si>
-  <si>
     <t>Finding ways to notice and evaluate the accuracy of your negative thoughts are key to feeling better.</t>
   </si>
   <si>
@@ -505,6 +499,18 @@
   </si>
   <si>
     <t xml:space="preserve">When we do behavioral experiments, we will create hypotheses to test. In “"ypothesis testing," we challenge unhelpful behaviors and thoughts by testing out alternative ways of responding. </t>
+  </si>
+  <si>
+    <t>For example, if you feel depressed, you will likely have many negative thoughts, possibly about yourself or others, or about your life in general.</t>
+  </si>
+  <si>
+    <t>cbt02_6</t>
+  </si>
+  <si>
+    <t>The first step in doing this is learning to catch or identify automatic thoughts.</t>
+  </si>
+  <si>
+    <t>Automatic thoughts are thoughts that pop into our heads, and most of the time, they happen automatically and outside of our awareness.</t>
   </si>
 </sst>
 </file>
@@ -563,8 +569,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -584,13 +594,17 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -920,10 +934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:B82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -949,634 +963,642 @@
     </row>
     <row r="3" spans="1:2" ht="30">
       <c r="A3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30">
       <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30">
       <c r="A7" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="30">
-      <c r="A8" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30">
       <c r="A9" s="2" t="s">
-        <v>121</v>
+        <v>163</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" t="s">
         <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30">
       <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
         <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30">
       <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="30">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
         <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="1" t="s">
-        <v>22</v>
+      <c r="A15" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
         <v>28</v>
-      </c>
-      <c r="B18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B19" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="30">
+      <c r="A23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="30">
-      <c r="A22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="1" t="s">
+      <c r="B26" t="s">
         <v>37</v>
-      </c>
-      <c r="B25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B26" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="27">
+      <c r="A30" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="27">
-      <c r="A29" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B30" t="s">
+    <row r="32" spans="1:2" ht="27">
+      <c r="A32" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B32" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="27">
-      <c r="A31" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B32" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="27">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" s="3" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="27">
       <c r="A36" s="3" t="s">
-        <v>125</v>
+        <v>159</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="27">
       <c r="A37" s="3" t="s">
-        <v>158</v>
+        <v>124</v>
       </c>
       <c r="B37" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="27">
       <c r="A38" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B38" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="27">
+      <c r="A39" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B40" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B39" t="s">
+    <row r="41" spans="1:2">
+      <c r="A41" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="1" t="s">
+      <c r="B41" t="s">
         <v>53</v>
       </c>
-      <c r="B40" t="s">
+    </row>
+    <row r="42" spans="1:2" ht="30">
+      <c r="A42" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="30">
-      <c r="A41" s="1" t="s">
+      <c r="B42" t="s">
         <v>55</v>
-      </c>
-      <c r="B41" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B42" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" t="s">
         <v>58</v>
       </c>
-      <c r="B43" t="s">
+    </row>
+    <row r="45" spans="1:2" ht="30">
+      <c r="A45" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="30">
-      <c r="A44" s="1" t="s">
+      <c r="B45" t="s">
         <v>60</v>
-      </c>
-      <c r="B44" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B45" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" t="s">
         <v>64</v>
-      </c>
-      <c r="B46" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="30">
-      <c r="A47" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B47" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="30">
       <c r="A48" s="1" t="s">
-        <v>127</v>
+        <v>65</v>
       </c>
       <c r="B48" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="30">
+      <c r="A49" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B49" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B50" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B49" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="30">
-      <c r="A50" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B50" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="30">
       <c r="A51" s="1" t="s">
-        <v>71</v>
+        <v>129</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="30">
       <c r="A52" s="1" t="s">
-        <v>131</v>
+        <v>70</v>
       </c>
       <c r="B52" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="30">
       <c r="A53" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B53" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="30">
       <c r="A54" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B54" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="30">
+      <c r="A55" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B55" t="s">
         <v>75</v>
       </c>
-      <c r="B54" t="s">
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B56" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B55" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="30">
-      <c r="A56" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B56" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="30">
       <c r="A57" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="30">
+      <c r="A58" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B58" t="s">
         <v>80</v>
       </c>
-      <c r="B57" t="s">
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B59" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B58" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="30">
-      <c r="A59" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B59" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="30">
       <c r="A60" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B60" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="30">
       <c r="A61" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B61" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="30">
+      <c r="A62" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B62" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="45">
+      <c r="A63" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B63" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="45">
-      <c r="A62" s="1" t="s">
+    <row r="64" spans="1:2">
+      <c r="A64" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B64" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="30">
+      <c r="A65" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B62" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B63" t="s">
+      <c r="B65" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="30">
-      <c r="A64" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B64" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B65" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B66" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B67" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B68" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="1" t="s">
-        <v>139</v>
+        <v>97</v>
       </c>
       <c r="B69" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B71" t="s">
         <v>101</v>
-      </c>
-      <c r="B70" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="30">
-      <c r="A71" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B71" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="30">
       <c r="A72" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B72" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="30">
+      <c r="A73" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B73" t="s">
         <v>105</v>
       </c>
-      <c r="B72" t="s">
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="1" t="s">
+      <c r="B74" t="s">
         <v>107</v>
-      </c>
-      <c r="B73" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="30">
-      <c r="A74" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B74" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="30">
       <c r="A75" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B75" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="30">
       <c r="A76" s="1" t="s">
-        <v>111</v>
+        <v>140</v>
       </c>
       <c r="B76" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="1" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
       <c r="B77" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B78" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B79" t="s">
         <v>114</v>
-      </c>
-      <c r="B78" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="45">
-      <c r="A79" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B79" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="45">
       <c r="A80" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B80" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="45">
+      <c r="A81" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B81" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="1" t="s">
+      <c r="B82" t="s">
         <v>118</v>
-      </c>
-      <c r="B81" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
split up longer chunks
</commit_message>
<xml_diff>
--- a/input/PROP_trialText.xlsx
+++ b/input/PROP_trialText.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="176">
   <si>
     <t>%stFile</t>
   </si>
@@ -378,12 +378,6 @@
     <t>pst10_5</t>
   </si>
   <si>
-    <t>When depressed, people frequently overlook their negative thoughts or cognitions, and assume what they are thinking is truth or reality. In therapy, we work to question the reality created by depressive thoughts.</t>
-  </si>
-  <si>
-    <t>We are usually more aware of the emotions these thoughts make us feel, such as sad or depressed, and we do not question what we are thinking. But often, the thoughts we are having are distorting reality in some way.</t>
-  </si>
-  <si>
     <t>Because your automatic thoughts are so quick, they are hard to notice or remember.</t>
   </si>
   <si>
@@ -393,66 +387,27 @@
     <t>Writing them down forces you to look at them more objectively.</t>
   </si>
   <si>
-    <t>We do this by developing a behavioral experiment to test if your new way of thinking or new behavior makes you feel better than your current thoughts and behaviors. We then "collect data" as you run the experiment.</t>
-  </si>
-  <si>
     <t>Using the SUDS, your emotions will range in intensity from 0 (not noticeable) to 100 (the highest extreme).</t>
   </si>
   <si>
     <t>The four skills are problem definition, generating alternatives, decision-making, and solution implementation and verification.</t>
   </si>
   <si>
-    <t>We want to practice identifying them by writing them down on what we call a "Thought Record."</t>
-  </si>
-  <si>
     <t>We usually notice how we're feeling before we notice what we're thinking.</t>
   </si>
   <si>
     <t>You will learn how to set a realistic problem-solving goal and identify the obstacles that are currently preventing you from reaching that goal.</t>
   </si>
   <si>
-    <t>One skill that may help you is the "generation of alternatives," in which we teach you to use your creative skills to brainstorm different types of solutions.</t>
-  </si>
-  <si>
-    <t>One skill that may help you is called "problem definition," or the clarifying the nature of a problem.</t>
-  </si>
-  <si>
     <t>You will come up with as many solutions as you can. Not all will be the best solution, but it helps you think of alternatives.</t>
   </si>
   <si>
-    <t>Using the skill of "decision making," you will learn how to look at the likely consequences of different solution ideas.</t>
-  </si>
-  <si>
-    <t>One skill that may help you is called "solution implementation and verification."</t>
-  </si>
-  <si>
-    <t>Through "externalization" you will experience how writing things down, recording messages for yourself on your iPhone, or talking through a difficult problem helps you to be less overwhelmed.</t>
-  </si>
-  <si>
-    <t>Try getting the brain overload you are experiencing with a difficult problem "out of your head" and onto paper, and you may notice that the thinking part of your brain can better understand and begin to organize this challenging problem or goal.</t>
-  </si>
-  <si>
     <t>Let's write down all of the thoughts, feelings, and concerns that are contributing to your experience of being overwhelmed as a way to begin to organize all of this information.</t>
   </si>
   <si>
-    <t>We teach you the use of "simplification" to break down a large or complex problem to make it more manageable.</t>
-  </si>
-  <si>
     <t>Try imagining what it would be like at a moment in time in the future when a stressful problem you are facing is largely resolved and the obstacles overcome, such as making a change in your plan for a career.</t>
   </si>
   <si>
-    <t>This won't immediately solve the problem but will give you an experience of what it would feel like to reach your goal and experience a "light at the end of the tunnel."</t>
-  </si>
-  <si>
-    <t>This important toolkit is referred to as the "SSTA" method.</t>
-  </si>
-  <si>
-    <t>The second S = Slow down and take a moment to "turn down the volume of strong emotions." You can take a few deep breaths, or use other techniques, so you can still listen to your feelings which give you important information, but allow your brain to keep working.</t>
-  </si>
-  <si>
-    <t>Ultimately, you will need to think carefully and planfully about an action plan that gives you the best chance of reaching your goals or solving a problem. Only after reducing intense emotional arousal and "turning down the volume," can you planfully and carefully.</t>
-  </si>
-  <si>
     <t>Also, when you're depressed, you're more likely to act in ways that feed your negative thoughts and sadness.</t>
   </si>
   <si>
@@ -468,9 +423,6 @@
     <t xml:space="preserve">By figuring out what cognitive distortions you may be having, you can respond to situations in a more healthy way. </t>
   </si>
   <si>
-    <t>One cognitive distortion is called "all or nothing thinking," where you see things in very black and white terms.</t>
-  </si>
-  <si>
     <t>For example, if you were feeling depressed and unable to finish your homework, you might think that you are a failure and will be a failure forever.</t>
   </si>
   <si>
@@ -486,21 +438,12 @@
     <t>We can then see if you do indeed feel worse as your automatic thought predicts you will.</t>
   </si>
   <si>
-    <t xml:space="preserve">Doing a "behavioral experiment" is one way to collect and examine the evidence. To do this, you may act out your automatic thought to see if what you predict happens. </t>
-  </si>
-  <si>
-    <t>For example, you know that avoiding your email is unhelpful for your depression. You have the hypothesis that checking your email will only worsen your mood and depression.</t>
-  </si>
-  <si>
     <t>You can then test out this hypothesis by checking your email at a specific time, and rating your mood before and after you checked your email.</t>
   </si>
   <si>
     <t>Once you've collected the data, we will evaluate the benefits of challenging your avoidance.</t>
   </si>
   <si>
-    <t xml:space="preserve">When we do behavioral experiments, we will create hypotheses to test. In “"ypothesis testing," we challenge unhelpful behaviors and thoughts by testing out alternative ways of responding. </t>
-  </si>
-  <si>
     <t>For example, if you feel depressed, you will likely have many negative thoughts, possibly about yourself or others, or about your life in general.</t>
   </si>
   <si>
@@ -511,6 +454,99 @@
   </si>
   <si>
     <t>Automatic thoughts are thoughts that pop into our heads, and most of the time, they happen automatically and outside of our awareness.</t>
+  </si>
+  <si>
+    <t>When depressed, people frequently overlook their negative thoughts or cognitions, and assume what they are thinking is truth or reality.</t>
+  </si>
+  <si>
+    <t>In therapy, we work to question the reality created by depressive thoughts.</t>
+  </si>
+  <si>
+    <t>But often, the thoughts we are having are distorting reality in some way.</t>
+  </si>
+  <si>
+    <t>We are usually more aware of the emotions these thoughts make us feel, such as sad or depressed, and we do not question what we are thinking.</t>
+  </si>
+  <si>
+    <t>cbt02_7</t>
+  </si>
+  <si>
+    <t>cbt02_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To do this, you may act out your automatic thought to see if what you predict happens. </t>
+  </si>
+  <si>
+    <t>cbt08_6</t>
+  </si>
+  <si>
+    <t>We do this by developing a behavioral experiment to test if your new way of thinking or new behavior makes you feel better than your current thoughts and behaviors.</t>
+  </si>
+  <si>
+    <t>cbt09_6</t>
+  </si>
+  <si>
+    <t>For example, you know that avoiding your email is unhelpful for your depression.</t>
+  </si>
+  <si>
+    <t>You have the hypothesis that checking your email will only worsen your mood and depression.</t>
+  </si>
+  <si>
+    <t>cbt09_7</t>
+  </si>
+  <si>
+    <t>We want to practice identifying them by writing them down on what we call a 'Thought Record.'</t>
+  </si>
+  <si>
+    <t>One cognitive distortion is called 'all or nothing thinking,' where you see things in very black and white terms.</t>
+  </si>
+  <si>
+    <t>Doing a 'behavioral experiment' is one way to collect and examine the evidence.</t>
+  </si>
+  <si>
+    <t>We then 'collect data' as you run the experiment.</t>
+  </si>
+  <si>
+    <t>One skill that may help you is called 'problem definition,' or the clarifying the nature of a problem.</t>
+  </si>
+  <si>
+    <t>One skill that may help you is the 'generation of alternatives,' in which we teach you to use your creative skills to brainstorm different types of solutions.</t>
+  </si>
+  <si>
+    <t>Using the skill of 'decision making,' you will learn how to look at the likely consequences of different solution ideas.</t>
+  </si>
+  <si>
+    <t>One skill that may help you is called 'solution implementation and verification.'</t>
+  </si>
+  <si>
+    <t>Through 'externalization' you will experience how writing things down, recording messages for yourself on your iPhone, or talking through a difficult problem helps you to be less overwhelmed.</t>
+  </si>
+  <si>
+    <t>Try getting the brain overload you are experiencing with a difficult problem 'out of your head' and onto paper, and you may notice that the thinking part of your brain can better understand and begin to organize this challenging problem or goal.</t>
+  </si>
+  <si>
+    <t>We teach you the use of 'simplification' to break down a large or complex problem to make it more manageable.</t>
+  </si>
+  <si>
+    <t>This won't immediately solve the problem but will give you an experience of what it would feel like to reach your goal and experience a 'light at the end of the tunnel.'</t>
+  </si>
+  <si>
+    <t>This important toolkit is referred to as the 'SSTA' method.</t>
+  </si>
+  <si>
+    <t>The second S = Slow down and take a moment to 'turn down the volume of strong emotions.' You can take a few deep breaths, or use other techniques, so you can still listen to your feelings which give you important information, but allow your brain to keep working.</t>
+  </si>
+  <si>
+    <t>Ultimately, you will need to think carefully and planfully about an action plan that gives you the best chance of reaching your goals or solving a problem. Only after reducing intense emotional arousal and 'turning down the volume,' can you planfully and carefully.</t>
+  </si>
+  <si>
+    <t>When we do behavioral experiments, we will create hypotheses to test.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In 'hypothesis testing,' we challenge unhelpful behaviors and thoughts by testing out alternative ways of responding. </t>
+  </si>
+  <si>
+    <t>cbt09_8</t>
   </si>
 </sst>
 </file>
@@ -569,8 +605,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -594,17 +640,27 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -934,10 +990,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B82"/>
+  <dimension ref="A1:B88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -963,7 +1019,7 @@
     </row>
     <row r="3" spans="1:2" ht="30">
       <c r="A3" s="1" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -971,7 +1027,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -995,7 +1051,7 @@
     </row>
     <row r="7" spans="1:2" ht="30">
       <c r="A7" s="2" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -1003,15 +1059,15 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="30">
+    <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
@@ -1019,585 +1075,633 @@
     </row>
     <row r="10" spans="1:2" ht="30">
       <c r="A10" s="2" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
+      <c r="A11" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="30">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
+    <row r="12" spans="1:2">
+      <c r="A12" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="B12" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="30">
       <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30">
+      <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B21" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="30">
-      <c r="A23" s="1" t="s">
+    <row r="25" spans="1:2" ht="30">
+      <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B23" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B28" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="3" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="27">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="3" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="3" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="27">
       <c r="A32" s="3" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="3" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="B33" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="3" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B37" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="27">
-      <c r="A36" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="38" spans="1:2">
+      <c r="A38" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B38" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B39" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="27">
-      <c r="A37" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B37" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="27">
-      <c r="A38" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B38" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="27">
-      <c r="A39" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B39" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="3" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="B40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="27">
+      <c r="A41" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B43" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B41" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="30">
-      <c r="A42" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B43" t="s">
-        <v>56</v>
-      </c>
-    </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="1" t="s">
-        <v>57</v>
+      <c r="A44" s="3" t="s">
+        <v>156</v>
       </c>
       <c r="B44" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="30">
-      <c r="A45" s="1" t="s">
-        <v>59</v>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="27">
+      <c r="A45" s="3" t="s">
+        <v>139</v>
       </c>
       <c r="B45" t="s">
-        <v>60</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="1" t="s">
-        <v>61</v>
+      <c r="A46" s="3" t="s">
+        <v>140</v>
       </c>
       <c r="B46" t="s">
-        <v>62</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B47" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="30">
       <c r="A48" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B48" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="30">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B49" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>131</v>
+        <v>57</v>
       </c>
       <c r="B50" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="30">
       <c r="A51" s="1" t="s">
-        <v>129</v>
+        <v>59</v>
       </c>
       <c r="B51" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="30">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B52" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="30">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
-        <v>130</v>
+        <v>63</v>
       </c>
       <c r="B53" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="30">
       <c r="A54" s="1" t="s">
-        <v>132</v>
+        <v>65</v>
       </c>
       <c r="B54" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="30">
       <c r="A55" s="1" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="B55" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="B56" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="30">
       <c r="A57" s="1" t="s">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="B57" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="30">
       <c r="A58" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B58" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="30">
       <c r="A59" s="1" t="s">
-        <v>134</v>
+        <v>163</v>
       </c>
       <c r="B59" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="30">
       <c r="A60" s="1" t="s">
-        <v>82</v>
+        <v>126</v>
       </c>
       <c r="B60" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="30">
       <c r="A61" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B61" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B62" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="30">
+      <c r="A63" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="30">
+      <c r="A64" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B64" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B65" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="30">
+      <c r="A66" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B66" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="30">
+      <c r="A67" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B67" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="30">
-      <c r="A62" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B62" t="s">
+    <row r="68" spans="1:2" ht="30">
+      <c r="A68" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B68" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="45">
-      <c r="A63" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B63" t="s">
+    <row r="69" spans="1:2" ht="45">
+      <c r="A69" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B69" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B64" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="30">
-      <c r="A65" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B65" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B66" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B67" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B68" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B69" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="1" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="B70" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="30">
       <c r="A71" s="1" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B71" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="30">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
       <c r="A72" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B72" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="30">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
       <c r="A73" s="1" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B73" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B74" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="30">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
       <c r="A75" s="1" t="s">
-        <v>139</v>
+        <v>97</v>
       </c>
       <c r="B75" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="30">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
       <c r="A76" s="1" t="s">
-        <v>140</v>
+        <v>168</v>
       </c>
       <c r="B76" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B77" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="30">
+      <c r="A78" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B78" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="30">
+      <c r="A79" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B79" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B80" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="30">
+      <c r="A81" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B81" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="30">
+      <c r="A82" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B82" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B83" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B78" t="s">
+    <row r="84" spans="1:2">
+      <c r="A84" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B84" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="1" t="s">
+    <row r="85" spans="1:2">
+      <c r="A85" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B85" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="45">
-      <c r="A80" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B80" t="s">
+    <row r="86" spans="1:2" ht="45">
+      <c r="A86" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B86" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="45">
-      <c r="A81" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B81" t="s">
+    <row r="87" spans="1:2" ht="45">
+      <c r="A87" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="1" t="s">
+    <row r="88" spans="1:2">
+      <c r="A88" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B88" t="s">
         <v>118</v>
       </c>
     </row>

</xml_diff>